<commit_message>
Added test for dates in other regions.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/PivotTables/PivotTableDateFormats.xlsx
+++ b/EPPlusTest/Workbooks/PivotTables/PivotTableDateFormats.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\EPPlus\EPPlusTest\Workbooks\PivotTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{657AE7DA-BAE2-42AD-B2FE-DC20D544DA63}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D70150-B070-44DE-B0C8-34B7B6EC86D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22824" windowHeight="10356" activeTab="2" xr2:uid="{5466E34F-AD35-41E8-9F27-92EF8590A682}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22824" windowHeight="10356" activeTab="3" xr2:uid="{5466E34F-AD35-41E8-9F27-92EF8590A682}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="RowFields" sheetId="2" r:id="rId2"/>
     <sheet name="ColumnFields" sheetId="3" r:id="rId3"/>
+    <sheet name="PivotTables" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="6" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="176">
   <si>
     <t>Address</t>
   </si>
@@ -569,7 +570,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="17">
+  <numFmts count="25">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="166" formatCode="m/d;@"/>
@@ -587,6 +588,14 @@
     <numFmt numFmtId="178" formatCode="[$-409]mmmmm\-yy;@"/>
     <numFmt numFmtId="179" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="180" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="183" formatCode="[$-10464]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="184" formatCode="d\.mm\.yy;@"/>
+    <numFmt numFmtId="185" formatCode="[$-1200C]d\ mmm\ yyyy;@"/>
+    <numFmt numFmtId="186" formatCode="[$-10478]yyyy&quot;ꈎ&quot;\ m&quot;ꆪ&quot;\ d&quot;ꑍ&quot;;@"/>
+    <numFmt numFmtId="187" formatCode="d\.\ m\.\ yy;@"/>
+    <numFmt numFmtId="188" formatCode="[$-10475]d\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="189" formatCode="[$-10470]dd/mm/yyyy;@"/>
+    <numFmt numFmtId="193" formatCode="[$-10488]dddd\ d\ mmmm\ yyyy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -617,7 +626,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -629,23 +638,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -697,17 +695,79 @@
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="186" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="188" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="189" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="193" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="95">
+  <dxfs count="171">
+    <dxf>
+      <numFmt numFmtId="190" formatCode="[$-60488]dddd\ d\ mmmm\ yyyy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="193" formatCode="[$-10488]dddd\ d\ mmmm\ yyyy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="188" formatCode="[$-10475]d\ mmmm\ yyyy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="189" formatCode="[$-10470]dd/mm/yyyy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="187" formatCode="d\.\ m\.\ yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="186" formatCode="[$-10478]yyyy&quot;ꈎ&quot;\ m&quot;ꆪ&quot;\ d&quot;ꑍ&quot;;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="185" formatCode="[$-1200C]d\ mmm\ yyyy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="184" formatCode="d\.mm\.yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="183" formatCode="[$-10464]mmmm\ d\,\ yyyy;@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     </dxf>
@@ -760,15 +820,168 @@
       <numFmt numFmtId="180" formatCode="[$-409]d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="m/d;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="m/d/yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="mm/dd/yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="[$-409]d\-mmm;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="[$-409]d\-mmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="171" formatCode="[$-409]dd\-mmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="172" formatCode="[$-409]mmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="173" formatCode="[$-409]mmmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="174" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="175" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode="m/d/yy\ h:mm;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="177" formatCode="[$-409]mmmmm;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="178" formatCode="[$-409]mmmmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="179" formatCode="m/d/yyyy;@"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="180" formatCode="[$-409]d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="m/d;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="m/d/yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="mm/dd/yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="[$-409]d\-mmm;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="[$-409]d\-mmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="171" formatCode="[$-409]dd\-mmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="172" formatCode="[$-409]mmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="173" formatCode="[$-409]mmmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="174" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="175" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode="m/d/yy\ h:mm;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="177" formatCode="[$-409]mmmmm;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="178" formatCode="[$-409]mmmmm\-yy;@"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="179" formatCode="m/d/yyyy;@"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="180" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="m/d;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="m/d/yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="mm/dd/yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="[$-409]d\-mmm;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="[$-409]d\-mmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="171" formatCode="[$-409]dd\-mmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="172" formatCode="[$-409]mmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="173" formatCode="[$-409]mmmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="174" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="175" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode="m/d/yy\ h:mm;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="177" formatCode="[$-409]mmmmm;@"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="178" formatCode="[$-409]mmmmm\-yy;@"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="179" formatCode="m/d/yyyy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="180" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="180" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="179" formatCode="m/d/yyyy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="178" formatCode="[$-409]mmmmm\-yy;@"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="177" formatCode="[$-409]mmmmm;@"/>
     </dxf>
     <dxf>
@@ -811,9 +1024,156 @@
       <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="m/d;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="m/d/yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="mm/dd/yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="[$-409]d\-mmm;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="[$-409]d\-mmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="171" formatCode="[$-409]dd\-mmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="172" formatCode="[$-409]mmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="172" formatCode="[$-409]mmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="174" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="175" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode="m/d/yy\ h:mm;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="177" formatCode="[$-409]mmmmm;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="178" formatCode="[$-409]mmmmm\-yy;@"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="180" formatCode="[$-409]d\-mmm\-yyyy;@"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="m/d;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="m/d/yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="mm/dd/yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="[$-409]d\-mmm;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="[$-409]d\-mmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="171" formatCode="[$-409]dd\-mmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="172" formatCode="[$-409]mmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="172" formatCode="[$-409]mmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="174" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="175" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode="m/d/yy\ h:mm;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="177" formatCode="[$-409]mmmmm;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="178" formatCode="[$-409]mmmmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="180" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="180" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="178" formatCode="[$-409]mmmmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="177" formatCode="[$-409]mmmmm;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode="m/d/yy\ h:mm;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="175" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="174" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="172" formatCode="[$-409]mmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="172" formatCode="[$-409]mmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="172" formatCode="[$-409]mmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="171" formatCode="[$-409]dd\-mmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="[$-409]d\-mmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="[$-409]d\-mmm;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="mm/dd/yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="m/d/yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="m/d;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="180" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="179" formatCode="m/d/yyyy;@"/>
     </dxf>
     <dxf>
@@ -847,106 +1207,7 @@
       <numFmt numFmtId="169" formatCode="[$-409]d\-mmm;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="mm/dd/yy;@"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="167" formatCode="m/d/yy;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="m/d;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="180" formatCode="[$-409]d\-mmm\-yyyy;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="179" formatCode="m/d/yyyy;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="178" formatCode="[$-409]mmmmm\-yy;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="177" formatCode="[$-409]mmmmm;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="176" formatCode="m/d/yy\ h:mm;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="175" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="174" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="173" formatCode="[$-409]mmmm\-yy;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="[$-409]mmm\-yy;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="[$-409]dd\-mmm\-yy;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="[$-409]d\-mmm\-yy;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="[$-409]d\-mmm;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="mm/dd/yy;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="m/d/yy;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="m/d;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="180" formatCode="[$-409]d\-mmm\-yyyy;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="179" formatCode="m/d/yyyy;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="178" formatCode="[$-409]mmmmm\-yy;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="177" formatCode="[$-409]mmmmm;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="176" formatCode="m/d/yy\ h:mm;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="175" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="174" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="173" formatCode="[$-409]mmmm\-yy;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="[$-409]mmm\-yy;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="[$-409]dd\-mmm\-yy;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="[$-409]d\-mmm\-yy;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="[$-409]d\-mmm;@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="168" formatCode="mm/dd/yy;@"/>
@@ -1388,753 +1649,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8AF0F2D4-142A-46EF-A8DC-CDCA657F88F7}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="E1:F23" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="10">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" numFmtId="14" showAll="0">
-      <items count="22">
-        <item x="10"/>
-        <item x="2"/>
-        <item x="9"/>
-        <item x="14"/>
-        <item x="17"/>
-        <item x="4"/>
-        <item x="13"/>
-        <item x="18"/>
-        <item x="8"/>
-        <item x="19"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item x="11"/>
-        <item x="15"/>
-        <item x="7"/>
-        <item x="1"/>
-        <item x="6"/>
-        <item x="16"/>
-        <item x="0"/>
-        <item x="20"/>
-        <item x="12"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="22">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Profit (LCY)" fld="9" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="17">
-    <format dxfId="50">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="49">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="48">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="47">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="46">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="45">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="44">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="43">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="8"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="42">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="9"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="41">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="10"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="40">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="11"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="39">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="12"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="38">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="13"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="37">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="14"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="36">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="15"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="35">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="16"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="34">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="17"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{12B01ED9-1547-42E5-9252-73B3E8A111E3}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A28:A93" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="10">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0">
-      <items count="23">
-        <item x="13"/>
-        <item x="5"/>
-        <item x="18"/>
-        <item x="17"/>
-        <item x="7"/>
-        <item x="19"/>
-        <item x="11"/>
-        <item x="0"/>
-        <item x="14"/>
-        <item x="4"/>
-        <item x="15"/>
-        <item x="9"/>
-        <item x="6"/>
-        <item x="21"/>
-        <item x="20"/>
-        <item x="10"/>
-        <item x="12"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="16"/>
-        <item x="8"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="22">
-        <item x="14"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="3"/>
-        <item x="16"/>
-        <item x="1"/>
-        <item x="12"/>
-        <item x="20"/>
-        <item x="17"/>
-        <item x="19"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="18"/>
-        <item x="13"/>
-        <item x="9"/>
-        <item x="15"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" numFmtId="14" subtotalTop="0" showAll="0">
-      <items count="22">
-        <item x="10"/>
-        <item x="2"/>
-        <item x="9"/>
-        <item x="14"/>
-        <item x="17"/>
-        <item x="4"/>
-        <item x="13"/>
-        <item x="18"/>
-        <item x="8"/>
-        <item x="19"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item x="11"/>
-        <item x="15"/>
-        <item x="7"/>
-        <item x="1"/>
-        <item x="6"/>
-        <item x="16"/>
-        <item x="0"/>
-        <item x="20"/>
-        <item x="12"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="3"/>
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="65">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i t="default">
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="18"/>
-    </i>
-    <i t="default">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="16"/>
-    </i>
-    <i t="default">
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i t="default">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i r="1">
-      <x v="10"/>
-    </i>
-    <i t="default">
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i t="default">
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="15"/>
-    </i>
-    <i t="default">
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i r="1">
-      <x v="14"/>
-    </i>
-    <i t="default">
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i r="1">
-      <x v="13"/>
-    </i>
-    <i t="default">
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i r="1">
-      <x v="11"/>
-    </i>
-    <i t="default">
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i t="default">
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i t="default">
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="4"/>
-    </i>
-    <i t="default">
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i r="1">
-      <x v="17"/>
-    </i>
-    <i t="default">
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i r="1">
-      <x v="12"/>
-    </i>
-    <i t="default">
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i t="default">
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i r="1">
-      <x v="20"/>
-    </i>
-    <i t="default">
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i t="default">
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i t="default">
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i r="1">
-      <x v="9"/>
-    </i>
-    <i t="default">
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i r="1">
-      <x v="8"/>
-    </i>
-    <i t="default">
-      <x v="20"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <formats count="17">
-    <format dxfId="67">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="66">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="65">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="64">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="63">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="62">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="61">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="60">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="8"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="59">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="9"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="58">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="10"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="57">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="11"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="56">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="12"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="55">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="13"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="54">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="14"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="53">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="15"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="52">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="16"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="51">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="17"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5BFA2560-73EA-4C6C-BACE-206D267B8550}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{46F993A9-86A4-4C1A-B744-4C4A7DD9EA12}" name="PivotTable4" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="E28:E137" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -2561,8 +2076,8 @@
   <colItems count="1">
     <i/>
   </colItems>
-  <formats count="17">
-    <format dxfId="84">
+  <formats count="16">
+    <format dxfId="110">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2571,7 +2086,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="83">
+    <format dxfId="111">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2580,7 +2095,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="82">
+    <format dxfId="112">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2589,7 +2104,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="81">
+    <format dxfId="113">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2598,7 +2113,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="80">
+    <format dxfId="114">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2607,7 +2122,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="79">
+    <format dxfId="115">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2616,7 +2131,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="78">
+    <format dxfId="116">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2625,7 +2140,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="77">
+    <format dxfId="117">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2634,7 +2149,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="76">
+    <format dxfId="118">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2643,7 +2158,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="75">
+    <format dxfId="119">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2652,7 +2167,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="74">
+    <format dxfId="120">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2661,7 +2176,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="73">
+    <format dxfId="121">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2670,7 +2185,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="72">
+    <format dxfId="122">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2679,7 +2194,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="71">
+    <format dxfId="123">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2688,7 +2203,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="70">
+    <format dxfId="124">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2697,16 +2212,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="69">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="16"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="68">
+    <format dxfId="125">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2728,8 +2234,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C491C702-9426-4788-B71C-EBDF4C63C70D}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C491C702-9426-4788-B71C-EBDF4C63C70D}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:B23" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
@@ -2857,8 +2363,745 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8AF0F2D4-142A-46EF-A8DC-CDCA657F88F7}" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="E1:F23" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" numFmtId="14" showAll="0">
+      <items count="22">
+        <item x="10"/>
+        <item x="2"/>
+        <item x="9"/>
+        <item x="14"/>
+        <item x="17"/>
+        <item x="4"/>
+        <item x="13"/>
+        <item x="18"/>
+        <item x="8"/>
+        <item x="19"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="11"/>
+        <item x="15"/>
+        <item x="7"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item x="16"/>
+        <item x="0"/>
+        <item x="20"/>
+        <item x="12"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="22">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Profit (LCY)" fld="9" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="17">
+    <format dxfId="160">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="159">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="158">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="157">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="156">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="154">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="153">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="152">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="151">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="150">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="149">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="11"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="148">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="12"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="147">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="13"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="146">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="14"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="145">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="15"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="144">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="16"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="143">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="17"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{12B01ED9-1547-42E5-9252-73B3E8A111E3}" name="PivotTable3" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A28:A93" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0">
+      <items count="23">
+        <item x="13"/>
+        <item x="5"/>
+        <item x="18"/>
+        <item x="17"/>
+        <item x="7"/>
+        <item x="19"/>
+        <item x="11"/>
+        <item x="0"/>
+        <item x="14"/>
+        <item x="4"/>
+        <item x="15"/>
+        <item x="9"/>
+        <item x="6"/>
+        <item x="21"/>
+        <item x="20"/>
+        <item x="10"/>
+        <item x="12"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="16"/>
+        <item x="8"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="22">
+        <item x="14"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="3"/>
+        <item x="16"/>
+        <item x="1"/>
+        <item x="12"/>
+        <item x="20"/>
+        <item x="17"/>
+        <item x="19"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="18"/>
+        <item x="13"/>
+        <item x="9"/>
+        <item x="15"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" numFmtId="14" subtotalTop="0" showAll="0">
+      <items count="22">
+        <item x="10"/>
+        <item x="2"/>
+        <item x="9"/>
+        <item x="14"/>
+        <item x="17"/>
+        <item x="4"/>
+        <item x="13"/>
+        <item x="18"/>
+        <item x="8"/>
+        <item x="19"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="11"/>
+        <item x="15"/>
+        <item x="7"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item x="16"/>
+        <item x="0"/>
+        <item x="20"/>
+        <item x="12"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="3"/>
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="65">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="18"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="16"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i t="default">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i t="default">
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="15"/>
+    </i>
+    <i t="default">
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="14"/>
+    </i>
+    <i t="default">
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="13"/>
+    </i>
+    <i t="default">
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="11"/>
+    </i>
+    <i t="default">
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i t="default">
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i t="default">
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i r="1">
+      <x v="17"/>
+    </i>
+    <i t="default">
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i r="1">
+      <x v="12"/>
+    </i>
+    <i t="default">
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i t="default">
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i r="1">
+      <x v="20"/>
+    </i>
+    <i t="default">
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i t="default">
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i t="default">
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
+    <i t="default">
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i t="default">
+      <x v="20"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <formats count="16">
+    <format dxfId="142">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="141">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="140">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="139">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="138">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="137">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="136">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="135">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="133">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="132">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="131">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="11"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="130">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="12"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="129">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="13"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="128">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="14"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="127">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="15"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="126">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="17"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0C95EC22-2453-4C6D-808E-BEC122B1E888}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B198C5B8-5E89-475D-A5B2-488FD5AE2A01}" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A31:AS56" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
@@ -3185,7 +3428,7 @@
     <dataField name="Sum of Profit (LCY)" fld="9" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="17">
-    <format dxfId="0">
+    <format dxfId="60">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3194,7 +3437,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="61">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3203,7 +3446,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="62">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3212,7 +3455,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="63">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3221,7 +3464,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="64">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3230,7 +3473,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="5">
+    <format dxfId="65">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3239,7 +3482,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="6">
+    <format dxfId="66">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3248,7 +3491,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="67">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3257,7 +3500,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="8">
+    <format dxfId="68">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3266,7 +3509,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="69">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3275,7 +3518,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="10">
+    <format dxfId="70">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3284,7 +3527,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="11">
+    <format dxfId="71">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3293,7 +3536,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="12">
+    <format dxfId="72">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3302,7 +3545,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="73">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3311,7 +3554,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="14">
+    <format dxfId="74">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3320,7 +3563,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="15">
+    <format dxfId="75">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3329,7 +3572,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="16">
+    <format dxfId="76">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3352,7 +3595,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{73E8B1F7-3D94-4E54-8850-1998653B75F7}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{73E8B1F7-3D94-4E54-8850-1998653B75F7}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:W25" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
@@ -3566,7 +3809,7 @@
     <dataField name="Sum of Profit (LCY)" fld="9" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="17">
-    <format dxfId="33">
+    <format dxfId="93">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3575,7 +3818,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="32">
+    <format dxfId="92">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3584,7 +3827,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="31">
+    <format dxfId="91">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3593,7 +3836,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="30">
+    <format dxfId="90">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3602,7 +3845,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="29">
+    <format dxfId="89">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3611,7 +3854,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="28">
+    <format dxfId="88">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3620,7 +3863,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="27">
+    <format dxfId="87">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3629,7 +3872,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="26">
+    <format dxfId="86">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3638,7 +3881,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="25">
+    <format dxfId="85">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3647,7 +3890,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="24">
+    <format dxfId="84">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3656,7 +3899,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="23">
+    <format dxfId="83">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3665,7 +3908,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="22">
+    <format dxfId="82">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3674,7 +3917,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="21">
+    <format dxfId="81">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3683,7 +3926,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="20">
+    <format dxfId="80">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3692,7 +3935,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="19">
+    <format dxfId="79">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3701,7 +3944,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="18">
+    <format dxfId="78">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3710,7 +3953,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="17">
+    <format dxfId="77">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -3732,20 +3975,249 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7363CFC3-2105-41A3-A461-22CC499C58BC}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:B23" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="23">
+        <item x="13"/>
+        <item x="5"/>
+        <item x="18"/>
+        <item x="17"/>
+        <item x="7"/>
+        <item x="19"/>
+        <item x="11"/>
+        <item x="0"/>
+        <item x="14"/>
+        <item x="4"/>
+        <item x="15"/>
+        <item x="9"/>
+        <item x="6"/>
+        <item x="21"/>
+        <item x="20"/>
+        <item x="10"/>
+        <item x="12"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="16"/>
+        <item x="8"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" numFmtId="14" showAll="0">
+      <items count="22">
+        <item x="10"/>
+        <item x="2"/>
+        <item x="9"/>
+        <item x="14"/>
+        <item x="17"/>
+        <item x="4"/>
+        <item x="13"/>
+        <item x="18"/>
+        <item x="8"/>
+        <item x="19"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="11"/>
+        <item x="15"/>
+        <item x="7"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item x="16"/>
+        <item x="0"/>
+        <item x="20"/>
+        <item x="12"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="22">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Profit (LCY)" fld="9" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="8">
+    <format dxfId="8">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="7">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="6">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="5">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="4">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="3">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="13"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="2">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="11"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="1">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="18"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B5B34B72-28FF-45A5-95B1-DFDA3B4A5F59}" name="table1" displayName="table1" ref="A1:J24" totalsRowCount="1">
   <autoFilter ref="A1:J23" xr:uid="{74FB4DD8-4789-4E12-90FE-DD4BB4181FF9}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{9E6DD651-A4A3-4AE7-8ADA-385E771697B5}" name="Address" totalsRowLabel="Total" dataDxfId="94"/>
-    <tableColumn id="2" xr3:uid="{6367AA86-704B-4B17-B5C0-F83546172382}" name="Name" dataDxfId="93"/>
-    <tableColumn id="3" xr3:uid="{094F912B-D913-4CE4-8BEE-4226C4D6A188}" name="City" dataDxfId="92"/>
-    <tableColumn id="4" xr3:uid="{AE25E532-41FB-4394-83A5-577BCDC98B9F}" name="Last Date Modified" dataDxfId="91"/>
-    <tableColumn id="5" xr3:uid="{209313FD-A9C1-4D35-9F5C-360DFAFA1808}" name="Contact" dataDxfId="90"/>
-    <tableColumn id="6" xr3:uid="{F6C57A65-3338-4572-9B46-8EE189772123}" name="Country/Region Code" dataDxfId="89"/>
-    <tableColumn id="7" xr3:uid="{F4EB61D7-6F11-4F5A-80A3-618AEF3D8A6C}" name="No." dataDxfId="88"/>
-    <tableColumn id="8" xr3:uid="{1D59407F-E7FB-4C0B-93C2-0511C707B778}" name="Net Change" totalsRowFunction="sum" dataDxfId="87"/>
-    <tableColumn id="9" xr3:uid="{98E69C1F-D69C-4DE0-A851-A974BA6FCF84}" name="Outstanding Orders" totalsRowFunction="sum" dataDxfId="86"/>
-    <tableColumn id="10" xr3:uid="{FD17C497-4EDB-4781-A2B6-EE4DFC531C14}" name="Profit (LCY)" totalsRowFunction="sum" dataDxfId="85"/>
+    <tableColumn id="1" xr3:uid="{9E6DD651-A4A3-4AE7-8ADA-385E771697B5}" name="Address" totalsRowLabel="Total" dataDxfId="170"/>
+    <tableColumn id="2" xr3:uid="{6367AA86-704B-4B17-B5C0-F83546172382}" name="Name" dataDxfId="169"/>
+    <tableColumn id="3" xr3:uid="{094F912B-D913-4CE4-8BEE-4226C4D6A188}" name="City" dataDxfId="168"/>
+    <tableColumn id="4" xr3:uid="{AE25E532-41FB-4394-83A5-577BCDC98B9F}" name="Last Date Modified" dataDxfId="167"/>
+    <tableColumn id="5" xr3:uid="{209313FD-A9C1-4D35-9F5C-360DFAFA1808}" name="Contact" dataDxfId="166"/>
+    <tableColumn id="6" xr3:uid="{F6C57A65-3338-4572-9B46-8EE189772123}" name="Country/Region Code" dataDxfId="165"/>
+    <tableColumn id="7" xr3:uid="{F4EB61D7-6F11-4F5A-80A3-618AEF3D8A6C}" name="No." dataDxfId="164"/>
+    <tableColumn id="8" xr3:uid="{1D59407F-E7FB-4C0B-93C2-0511C707B778}" name="Net Change" totalsRowFunction="sum" dataDxfId="163"/>
+    <tableColumn id="9" xr3:uid="{98E69C1F-D69C-4DE0-A851-A974BA6FCF84}" name="Outstanding Orders" totalsRowFunction="sum" dataDxfId="162"/>
+    <tableColumn id="10" xr3:uid="{FD17C497-4EDB-4781-A2B6-EE4DFC531C14}" name="Profit (LCY)" totalsRowFunction="sum" dataDxfId="161"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4821,8 +5293,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A958A5-D4FF-4C91-892E-A6868B5BAE45}">
   <dimension ref="A1:F137"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E114" sqref="E114"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E35" activeCellId="1" sqref="E30 E35 E40 E45 E50 E55 E60 E65 E70 E75 E80 E85 E90 E93 E98 E103 E108 E113 E118 E123 E128 E133"/>
+      <pivotSelection pane="bottomRight" showHeader="1" axis="axisRow" dimension="1" activeRow="34" activeCol="4" previousRow="34" previousCol="4" click="1" r:id="rId1">
+        <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+          <references count="1">
+            <reference field="2" count="0"/>
+          </references>
+        </pivotArea>
+      </pivotSelection>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4885,7 +5364,7 @@
       <c r="B3" s="3">
         <v>0</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="9">
         <v>40943</v>
       </c>
       <c r="F3" s="3">
@@ -4899,7 +5378,7 @@
       <c r="B4" s="3">
         <v>0</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="10">
         <v>40958</v>
       </c>
       <c r="F4" s="3">
@@ -4913,7 +5392,7 @@
       <c r="B5" s="3">
         <v>0</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="11">
         <v>40959</v>
       </c>
       <c r="F5" s="3">
@@ -4927,7 +5406,7 @@
       <c r="B6" s="3">
         <v>95.410000000000011</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="12">
         <v>40965</v>
       </c>
       <c r="F6" s="3">
@@ -4941,7 +5420,7 @@
       <c r="B7" s="3">
         <v>0</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="13">
         <v>40967</v>
       </c>
       <c r="F7" s="3">
@@ -4955,7 +5434,7 @@
       <c r="B8" s="3">
         <v>0</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="14">
         <v>41043</v>
       </c>
       <c r="F8" s="3">
@@ -4969,7 +5448,7 @@
       <c r="B9" s="3">
         <v>0</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="15">
         <v>41048</v>
       </c>
       <c r="F9" s="3">
@@ -4983,7 +5462,7 @@
       <c r="B10" s="3">
         <v>0</v>
       </c>
-      <c r="E10" s="31">
+      <c r="E10" s="16">
         <v>41050</v>
       </c>
       <c r="F10" s="3">
@@ -4997,7 +5476,7 @@
       <c r="B11" s="3">
         <v>0</v>
       </c>
-      <c r="E11" s="32">
+      <c r="E11" s="17">
         <v>41052</v>
       </c>
       <c r="F11" s="3">
@@ -5011,7 +5490,7 @@
       <c r="B12" s="3">
         <v>0</v>
       </c>
-      <c r="E12" s="33">
+      <c r="E12" s="18">
         <v>41055</v>
       </c>
       <c r="F12" s="3">
@@ -5025,7 +5504,7 @@
       <c r="B13" s="3">
         <v>1119.44</v>
       </c>
-      <c r="E13" s="34">
+      <c r="E13" s="19">
         <v>41125</v>
       </c>
       <c r="F13" s="3">
@@ -5039,7 +5518,7 @@
       <c r="B14" s="3">
         <v>546</v>
       </c>
-      <c r="E14" s="35">
+      <c r="E14" s="20">
         <v>41127</v>
       </c>
       <c r="F14" s="3">
@@ -5053,7 +5532,7 @@
       <c r="B15" s="3">
         <v>334.27000000000004</v>
       </c>
-      <c r="E15" s="36">
+      <c r="E15" s="21">
         <v>41137</v>
       </c>
       <c r="F15" s="3">
@@ -5067,7 +5546,7 @@
       <c r="B16" s="3">
         <v>0</v>
       </c>
-      <c r="E16" s="37">
+      <c r="E16" s="22">
         <v>41138</v>
       </c>
       <c r="F16" s="3">
@@ -5081,7 +5560,7 @@
       <c r="B17" s="3">
         <v>0</v>
       </c>
-      <c r="E17" s="38">
+      <c r="E17" s="23">
         <v>41147</v>
       </c>
       <c r="F17" s="3">
@@ -5095,7 +5574,7 @@
       <c r="B18" s="3">
         <v>0</v>
       </c>
-      <c r="E18" s="39">
+      <c r="E18" s="24">
         <v>41155</v>
       </c>
       <c r="F18" s="3">
@@ -5109,7 +5588,7 @@
       <c r="B19" s="3">
         <v>0</v>
       </c>
-      <c r="E19" s="40">
+      <c r="E19" s="25">
         <v>41161</v>
       </c>
       <c r="F19" s="3">
@@ -5192,10 +5671,10 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="41" t="s">
+      <c r="A30" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="E30" s="41" t="s">
+      <c r="E30" s="7" t="s">
         <v>70</v>
       </c>
     </row>
@@ -5203,20 +5682,20 @@
       <c r="A31" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="E31" s="42" t="s">
+      <c r="E31" s="8" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="24">
+      <c r="A32" s="9">
         <v>40943</v>
       </c>
-      <c r="E32" s="41" t="s">
+      <c r="E32" s="7" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="41" t="s">
+      <c r="A33" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E33" s="5" t="s">
@@ -5227,23 +5706,23 @@
       <c r="A34" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="E34" s="24">
+      <c r="E34" s="9">
         <v>40943</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="25">
+      <c r="A35" s="10">
         <v>40958</v>
       </c>
-      <c r="E35" s="41" t="s">
+      <c r="E35" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="41" t="s">
+      <c r="A36" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E36" s="42" t="s">
+      <c r="E36" s="8" t="s">
         <v>22</v>
       </c>
     </row>
@@ -5251,12 +5730,12 @@
       <c r="A37" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E37" s="41" t="s">
+      <c r="E37" s="7" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="26">
+      <c r="A38" s="11">
         <v>40959</v>
       </c>
       <c r="E38" s="5" t="s">
@@ -5264,10 +5743,10 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="41" t="s">
+      <c r="A39" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="E39" s="25">
+      <c r="E39" s="10">
         <v>40958</v>
       </c>
     </row>
@@ -5275,23 +5754,23 @@
       <c r="A40" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="E40" s="41" t="s">
+      <c r="E40" s="7" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="27">
+      <c r="A41" s="12">
         <v>40965</v>
       </c>
-      <c r="E41" s="42" t="s">
+      <c r="E41" s="8" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="41" t="s">
+      <c r="A42" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="E42" s="41" t="s">
+      <c r="E42" s="7" t="s">
         <v>171</v>
       </c>
     </row>
@@ -5304,18 +5783,18 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="28">
+      <c r="A44" s="13">
         <v>40967</v>
       </c>
-      <c r="E44" s="26">
+      <c r="E44" s="11">
         <v>40959</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="41" t="s">
+      <c r="A45" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E45" s="41" t="s">
+      <c r="E45" s="7" t="s">
         <v>94</v>
       </c>
     </row>
@@ -5323,20 +5802,20 @@
       <c r="A46" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="E46" s="42" t="s">
+      <c r="E46" s="8" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="29">
+      <c r="A47" s="14">
         <v>41043</v>
       </c>
-      <c r="E47" s="41" t="s">
+      <c r="E47" s="7" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="41" t="s">
+      <c r="A48" s="7" t="s">
         <v>88</v>
       </c>
       <c r="E48" s="5" t="s">
@@ -5347,23 +5826,23 @@
       <c r="A49" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="E49" s="27">
+      <c r="E49" s="12">
         <v>40965</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="30">
+      <c r="A50" s="15">
         <v>41048</v>
       </c>
-      <c r="E50" s="41" t="s">
+      <c r="E50" s="7" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="41" t="s">
+      <c r="A51" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="E51" s="42" t="s">
+      <c r="E51" s="8" t="s">
         <v>114</v>
       </c>
     </row>
@@ -5371,12 +5850,12 @@
       <c r="A52" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="E52" s="41" t="s">
+      <c r="E52" s="7" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="31">
+      <c r="A53" s="16">
         <v>41050</v>
       </c>
       <c r="E53" s="5" t="s">
@@ -5384,10 +5863,10 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="41" t="s">
+      <c r="A54" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E54" s="28">
+      <c r="E54" s="13">
         <v>40967</v>
       </c>
     </row>
@@ -5395,23 +5874,23 @@
       <c r="A55" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="E55" s="41" t="s">
+      <c r="E55" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="32">
+      <c r="A56" s="17">
         <v>41052</v>
       </c>
-      <c r="E56" s="42" t="s">
+      <c r="E56" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="41" t="s">
+      <c r="A57" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="E57" s="41" t="s">
+      <c r="E57" s="7" t="s">
         <v>156</v>
       </c>
     </row>
@@ -5424,18 +5903,18 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="33">
+      <c r="A59" s="17">
         <v>41055</v>
       </c>
-      <c r="E59" s="29">
+      <c r="E59" s="14">
         <v>41043</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="41" t="s">
+      <c r="A60" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E60" s="41" t="s">
+      <c r="E60" s="7" t="s">
         <v>88</v>
       </c>
     </row>
@@ -5443,20 +5922,20 @@
       <c r="A61" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="E61" s="42" t="s">
+      <c r="E61" s="8" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="34">
+      <c r="A62" s="19">
         <v>41125</v>
       </c>
-      <c r="E62" s="41" t="s">
+      <c r="E62" s="7" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" s="41" t="s">
+      <c r="A63" s="7" t="s">
         <v>41</v>
       </c>
       <c r="E63" s="5" t="s">
@@ -5467,31 +5946,31 @@
       <c r="A64" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="E64" s="30">
+      <c r="E64" s="15">
         <v>41048</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="35">
+      <c r="A65" s="20">
         <v>41127</v>
       </c>
-      <c r="E65" s="41" t="s">
+      <c r="E65" s="7" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="41" t="s">
+      <c r="A66" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="E66" s="42" t="s">
+      <c r="E66" s="8" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" s="41" t="s">
+      <c r="A67" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="E67" s="41" t="s">
+      <c r="E67" s="7" t="s">
         <v>169</v>
       </c>
     </row>
@@ -5504,18 +5983,18 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" s="36">
+      <c r="A69" s="21">
         <v>41137</v>
       </c>
-      <c r="E69" s="31">
+      <c r="E69" s="16">
         <v>41050</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" s="41" t="s">
+      <c r="A70" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E70" s="41" t="s">
+      <c r="E70" s="7" t="s">
         <v>59</v>
       </c>
     </row>
@@ -5523,20 +6002,20 @@
       <c r="A71" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="E71" s="42" t="s">
+      <c r="E71" s="8" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" s="37">
+      <c r="A72" s="22">
         <v>41138</v>
       </c>
-      <c r="E72" s="41" t="s">
+      <c r="E72" s="7" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A73" s="41" t="s">
+      <c r="A73" s="7" t="s">
         <v>53</v>
       </c>
       <c r="E73" s="5" t="s">
@@ -5547,23 +6026,23 @@
       <c r="A74" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="E74" s="32">
+      <c r="E74" s="17">
         <v>41052</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" s="38">
+      <c r="A75" s="23">
         <v>41147</v>
       </c>
-      <c r="E75" s="41" t="s">
+      <c r="E75" s="7" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A76" s="41" t="s">
+      <c r="A76" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E76" s="42" t="s">
+      <c r="E76" s="8" t="s">
         <v>122</v>
       </c>
     </row>
@@ -5571,12 +6050,12 @@
       <c r="A77" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="E77" s="41" t="s">
+      <c r="E77" s="7" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A78" s="39">
+      <c r="A78" s="5">
         <v>41155</v>
       </c>
       <c r="E78" s="5" t="s">
@@ -5584,10 +6063,10 @@
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A79" s="41" t="s">
+      <c r="A79" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E79" s="33">
+      <c r="E79" s="17">
         <v>41055</v>
       </c>
     </row>
@@ -5595,23 +6074,23 @@
       <c r="A80" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="E80" s="41" t="s">
+      <c r="E80" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A81" s="40">
+      <c r="A81" s="25">
         <v>41161</v>
       </c>
-      <c r="E81" s="42" t="s">
+      <c r="E81" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A82" s="41" t="s">
+      <c r="A82" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="E82" s="41" t="s">
+      <c r="E82" s="7" t="s">
         <v>160</v>
       </c>
     </row>
@@ -5627,15 +6106,15 @@
       <c r="A84" s="5">
         <v>41165</v>
       </c>
-      <c r="E84" s="34">
+      <c r="E84" s="19">
         <v>41125</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A85" s="41" t="s">
+      <c r="A85" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E85" s="41" t="s">
+      <c r="E85" s="7" t="s">
         <v>41</v>
       </c>
     </row>
@@ -5643,7 +6122,7 @@
       <c r="A86" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="E86" s="42" t="s">
+      <c r="E86" s="8" t="s">
         <v>40</v>
       </c>
     </row>
@@ -5651,12 +6130,12 @@
       <c r="A87" s="5">
         <v>41176</v>
       </c>
-      <c r="E87" s="41" t="s">
+      <c r="E87" s="7" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A88" s="41" t="s">
+      <c r="A88" s="7" t="s">
         <v>127</v>
       </c>
       <c r="E88" s="5" t="s">
@@ -5667,7 +6146,7 @@
       <c r="A89" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="E89" s="35">
+      <c r="E89" s="20">
         <v>41127</v>
       </c>
     </row>
@@ -5675,15 +6154,15 @@
       <c r="A90" s="5">
         <v>41177</v>
       </c>
-      <c r="E90" s="41" t="s">
+      <c r="E90" s="7" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A91" s="41" t="s">
+      <c r="A91" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E91" s="42" t="s">
+      <c r="E91" s="8" t="s">
         <v>93</v>
       </c>
     </row>
@@ -5691,7 +6170,7 @@
       <c r="A92" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="E92" s="41" t="s">
+      <c r="E92" s="7" t="s">
         <v>155</v>
       </c>
     </row>
@@ -5699,17 +6178,17 @@
       <c r="A93" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="E93" s="41" t="s">
+      <c r="E93" s="7" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E94" s="42" t="s">
+      <c r="E94" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E95" s="41" t="s">
+      <c r="E95" s="7" t="s">
         <v>159</v>
       </c>
     </row>
@@ -5719,22 +6198,22 @@
       </c>
     </row>
     <row r="97" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E97" s="36">
+      <c r="E97" s="21">
         <v>41137</v>
       </c>
     </row>
     <row r="98" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E98" s="41" t="s">
+      <c r="E98" s="7" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="99" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E99" s="42" t="s">
+      <c r="E99" s="8" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="100" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E100" s="41" t="s">
+      <c r="E100" s="7" t="s">
         <v>172</v>
       </c>
     </row>
@@ -5744,22 +6223,22 @@
       </c>
     </row>
     <row r="102" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E102" s="37">
+      <c r="E102" s="22">
         <v>41138</v>
       </c>
     </row>
     <row r="103" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E103" s="41" t="s">
+      <c r="E103" s="7" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="104" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E104" s="42" t="s">
+      <c r="E104" s="8" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="105" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E105" s="41" t="s">
+      <c r="E105" s="7" t="s">
         <v>167</v>
       </c>
     </row>
@@ -5769,22 +6248,22 @@
       </c>
     </row>
     <row r="107" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E107" s="38">
+      <c r="E107" s="23">
         <v>41147</v>
       </c>
     </row>
     <row r="108" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E108" s="41" t="s">
+      <c r="E108" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="109" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E109" s="42" t="s">
+      <c r="E109" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="110" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E110" s="41" t="s">
+      <c r="E110" s="7" t="s">
         <v>162</v>
       </c>
     </row>
@@ -5794,22 +6273,22 @@
       </c>
     </row>
     <row r="112" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E112" s="39">
+      <c r="E112" s="5">
         <v>41155</v>
       </c>
     </row>
     <row r="113" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E113" s="41" t="s">
+      <c r="E113" s="7" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="114" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E114" s="42" t="s">
+      <c r="E114" s="8" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="115" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E115" s="41" t="s">
+      <c r="E115" s="7" t="s">
         <v>175</v>
       </c>
     </row>
@@ -5819,22 +6298,22 @@
       </c>
     </row>
     <row r="117" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E117" s="40">
+      <c r="E117" s="25">
         <v>41161</v>
       </c>
     </row>
     <row r="118" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E118" s="41" t="s">
+      <c r="E118" s="7" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="119" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E119" s="42" t="s">
+      <c r="E119" s="8" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="120" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E120" s="41" t="s">
+      <c r="E120" s="7" t="s">
         <v>161</v>
       </c>
     </row>
@@ -5849,17 +6328,17 @@
       </c>
     </row>
     <row r="123" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E123" s="41" t="s">
+      <c r="E123" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="124" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E124" s="42" t="s">
+      <c r="E124" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="125" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E125" s="41" t="s">
+      <c r="E125" s="7" t="s">
         <v>174</v>
       </c>
     </row>
@@ -5874,17 +6353,17 @@
       </c>
     </row>
     <row r="128" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E128" s="41" t="s">
+      <c r="E128" s="7" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="129" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E129" s="42" t="s">
+      <c r="E129" s="8" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="130" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E130" s="41" t="s">
+      <c r="E130" s="7" t="s">
         <v>164</v>
       </c>
     </row>
@@ -5899,17 +6378,17 @@
       </c>
     </row>
     <row r="133" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E133" s="41" t="s">
+      <c r="E133" s="7" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="134" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E134" s="42" t="s">
+      <c r="E134" s="8" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="135" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E135" s="41" t="s">
+      <c r="E135" s="7" t="s">
         <v>163</v>
       </c>
     </row>
@@ -5933,15 +6412,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8DFC673-DB69-4CFD-8083-8FDF2C262E08}">
   <dimension ref="A1:AS56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG16" workbookViewId="0">
-      <selection activeCell="Y32" sqref="Y32"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
@@ -5984,6 +6463,10 @@
     <col min="43" max="43" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
@@ -6001,55 +6484,55 @@
       <c r="B2" s="2">
         <v>40940</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="26">
         <v>40943</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="27">
         <v>40958</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="28">
         <v>40959</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="29">
         <v>40965</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="30">
         <v>40967</v>
       </c>
-      <c r="H2" s="12">
+      <c r="H2" s="31">
         <v>41043</v>
       </c>
-      <c r="I2" s="13">
+      <c r="I2" s="32">
         <v>41048</v>
       </c>
-      <c r="J2" s="14">
+      <c r="J2" s="33">
         <v>41050</v>
       </c>
-      <c r="K2" s="15">
+      <c r="K2" s="34">
         <v>41052</v>
       </c>
-      <c r="L2" s="16">
+      <c r="L2" s="35">
         <v>41055</v>
       </c>
-      <c r="M2" s="17">
+      <c r="M2" s="36">
         <v>41125</v>
       </c>
-      <c r="N2" s="18">
+      <c r="N2" s="37">
         <v>41127</v>
       </c>
-      <c r="O2" s="19">
+      <c r="O2" s="38">
         <v>41137</v>
       </c>
-      <c r="P2" s="20">
+      <c r="P2" s="39">
         <v>41138</v>
       </c>
-      <c r="Q2" s="21">
+      <c r="Q2" s="40">
         <v>41147</v>
       </c>
-      <c r="R2" s="22">
+      <c r="R2" s="41">
         <v>41155</v>
       </c>
-      <c r="S2" s="23">
+      <c r="S2" s="42">
         <v>41161</v>
       </c>
       <c r="T2" s="2">
@@ -6833,104 +7316,104 @@
       <c r="C32" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="26">
         <v>40943</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="F32" s="8">
+      <c r="F32" s="27">
         <v>40958</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="H32" s="9">
+      <c r="H32" s="28">
         <v>40959</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="J32" s="10">
+      <c r="J32" s="29">
         <v>40965</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="L32" s="11">
+      <c r="L32" s="30">
         <v>40967</v>
       </c>
       <c r="M32" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="N32" s="12">
+      <c r="N32" s="31">
         <v>41043</v>
       </c>
       <c r="O32" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="P32" s="13">
+      <c r="P32" s="32">
         <v>41048</v>
       </c>
       <c r="Q32" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="R32" s="14">
+      <c r="R32" s="33">
         <v>41050</v>
       </c>
       <c r="S32" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="T32" s="15">
+      <c r="T32" s="34">
         <v>41052</v>
       </c>
       <c r="U32" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="V32" s="16">
+      <c r="V32" s="35">
         <v>41055</v>
       </c>
       <c r="W32" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="X32" s="17">
+      <c r="X32" s="36">
         <v>41125</v>
       </c>
       <c r="Y32" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="Z32" s="18">
+      <c r="Z32" s="37">
         <v>41127</v>
       </c>
-      <c r="AA32" s="18"/>
+      <c r="AA32" s="37"/>
       <c r="AB32" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="AC32" s="19">
+      <c r="AC32" s="38">
         <v>41137</v>
       </c>
       <c r="AD32" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="AE32" s="20">
+      <c r="AE32" s="39">
         <v>41138</v>
       </c>
       <c r="AF32" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="AG32" s="21">
+      <c r="AG32" s="40">
         <v>41147</v>
       </c>
       <c r="AH32" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="AI32" s="22">
+      <c r="AI32" s="41">
         <v>41155</v>
       </c>
       <c r="AJ32" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="AK32" s="23">
+      <c r="AK32" s="42">
         <v>41161</v>
       </c>
       <c r="AL32" s="2" t="s">
@@ -8379,4 +8862,207 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4AE3C57-DC79-418F-AD1D-05CCF7B9F922}">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="43">
+        <v>40940</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1638.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="44">
+        <v>40943</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="45">
+        <v>40958</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="46">
+        <v>40959</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="47">
+        <v>40965</v>
+      </c>
+      <c r="B6" s="3">
+        <v>95.410000000000011</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>40967</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <v>41043</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>41048</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>41050</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>41052</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
+        <v>41055</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="48">
+        <v>41125</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1119.44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>41127</v>
+      </c>
+      <c r="B14" s="3">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="49">
+        <v>41137</v>
+      </c>
+      <c r="B15" s="3">
+        <v>334.27000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
+        <v>41138</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
+        <v>41147</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="5">
+        <v>41155</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
+        <v>41161</v>
+      </c>
+      <c r="B19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="50">
+        <v>41165</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
+        <v>41176</v>
+      </c>
+      <c r="B21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
+        <v>41177</v>
+      </c>
+      <c r="B22" s="3">
+        <v>847.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B23" s="3">
+        <v>4580.42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>